<commit_message>
Changes in TestNG.xml, upgrading Maven Surefire plugin
</commit_message>
<xml_diff>
--- a/src/Terms.xlsx
+++ b/src/Terms.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Google</t>
   </si>
@@ -28,6 +28,15 @@
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>Pasant</t>
+  </si>
+  <si>
+    <t>Suzan</t>
+  </si>
+  <si>
+    <t>Johnathan</t>
   </si>
 </sst>
 </file>
@@ -345,13 +354,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -366,6 +378,21 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>